<commit_message>
diagnostics file for toypam and the regression test updated so that kcat_b is taken into account, all test cases passed
</commit_message>
<xml_diff>
--- a/tests/data/diagnostics_file_for_toy.xlsx
+++ b/tests/data/diagnostics_file_for_toy.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\PAModelpy_\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91EBC68-44C9-4826-945F-8711D52DBE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D673AD5-107B-4350-BC88-D6A926B3B7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3825" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-11130" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
     <sheet name="case_01" sheetId="1" r:id="rId2"/>
     <sheet name="case_02" sheetId="3" r:id="rId3"/>
+    <sheet name="case_03" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="33">
   <si>
     <t>run_id</t>
   </si>
@@ -117,6 +118,15 @@
   </si>
   <si>
     <t>R5</t>
+  </si>
+  <si>
+    <t>case_03</t>
+  </si>
+  <si>
+    <t>same as case 1, but include backward reactions</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -440,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27796147-D834-40F8-8E40-5B811C63E8F1}">
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,6 +477,14 @@
       </c>
       <c r="B4" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -771,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2052CEE-0E47-4214-BD82-22E63BD76D32}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1057,4 +1075,296 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DD5CD7-6EC0-4341-B267-6758880451AA}">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <v>1015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>